<commit_message>
removed Mobile number from data base
</commit_message>
<xml_diff>
--- a/TestData/TestDataExcel_HotStar.xlsx
+++ b/TestData/TestDataExcel_HotStar.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ankitgupta/Desktop/Eclipse_Workspace/Ankit_Automation/Ankit_TestFrameWork/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ankitgupta/Desktop/Eclipse_Workspace/Ankit_Automation/HotStarProject/DemoHotStarProject/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67157215-1013-A348-B9D9-EF5AC2C54789}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CCCDFC-4EF4-FA40-B473-5FEBAE8BB055}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>SN</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>hotStar_Login</t>
+  </si>
+  <si>
+    <t>xxxxxxxxxx</t>
   </si>
 </sst>
 </file>
@@ -749,7 +752,7 @@
   <dimension ref="A1:AO43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -837,11 +840,11 @@
       <c r="B2" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
-        <v>7838198831</v>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D2" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="1"/>
@@ -882,7 +885,7 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="20"/>

</xml_diff>